<commit_message>
manifest updated; excel sheet minor edit
</commit_message>
<xml_diff>
--- a/data/funding_data1.xlsx
+++ b/data/funding_data1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Apple_Agroforestry\Apple_Agroforestry\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Walnut_Agroforestry\belgium_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3AABB5-5E2F-4676-931F-1DA316F969E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFF4FC6-059E-4ED2-A8F4-419C76C2DCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -62,6 +63,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -78,6 +80,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -94,6 +97,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -110,6 +114,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -126,6 +131,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Supported by Govt Forestry Commission Agroforestry Woodland Officers
@@ -140,6 +146,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Free bespoke design advice from Woodland Trust agroforestry advisors
@@ -164,6 +171,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -180,6 +188,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -196,6 +205,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -212,6 +222,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -228,6 +239,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -244,6 +256,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -260,6 +273,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Supported by Govt Forestry Commission Agroforestry Woodland Officers
@@ -274,6 +288,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Free bespoke design advice from Woodland Trust agroforestry advisors
@@ -286,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="248">
   <si>
     <t>Country</t>
   </si>
@@ -866,6 +881,7 @@
         <sz val="11"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Aanplantsubsidie voor boslandbouwsystemen (agroforestry) | Landbouw en Zeevisserij (vlaanderen.be)</t>
     </r>
@@ -877,6 +893,7 @@
         <sz val="11"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>VLIF Niet-productieve investeringen voor milieu- en klimaatdoelen | Landbouw en Zeevisserij (vlaanderen.be)</t>
     </r>
@@ -1045,6 +1062,9 @@
   </si>
   <si>
     <t>funding_onetime_per_m_hedgerow_schemes_c</t>
+  </si>
+  <si>
+    <t>Planting subsidy for new agroforestry plots (as per Agromilieu Klimaatmaatregelen (AMKM))</t>
   </si>
 </sst>
 </file>
@@ -1084,12 +1104,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1100,6 +1122,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1107,6 +1130,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1143,12 +1167,14 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1651,7 +1677,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1712,8 +1738,8 @@
       <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>186</v>
+      <c r="E2" s="42" t="s">
+        <v>247</v>
       </c>
       <c r="F2" s="6">
         <v>0.75</v>

</xml_diff>